<commit_message>
updated excel file to include condformat activity
</commit_message>
<xml_diff>
--- a/images/IntroExcelSampleWorkbook.xlsx
+++ b/images/IntroExcelSampleWorkbook.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\UI Library\Liaison Work\Library Instruction\Library Workshops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\GitHub\Git\intro-excel\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="7665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Charts" sheetId="6" r:id="rId2"/>
     <sheet name="Tricks" sheetId="7" r:id="rId3"/>
+    <sheet name="CondFormat" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$10</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
   <si>
     <t>Pennsylvania</t>
   </si>
@@ -127,7 +128,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -429,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -851,7 +908,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,4 +1131,235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>850</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2">
+        <f>SUM(C2:D2)</f>
+        <v>1350</v>
+      </c>
+      <c r="F2" s="2">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>950</v>
+      </c>
+      <c r="D3">
+        <v>475</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">SUM(C3:D3)</f>
+        <v>1425</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>695</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>995</v>
+      </c>
+      <c r="F4" s="2">
+        <v>41672</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <v>700</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="F5" s="2">
+        <v>40763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="D6">
+        <v>450</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1450</v>
+      </c>
+      <c r="F6" s="2">
+        <v>38721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1200</v>
+      </c>
+      <c r="D7">
+        <v>900</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="F7" s="2">
+        <v>36623</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>250</v>
+      </c>
+      <c r="D8">
+        <v>575</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>825</v>
+      </c>
+      <c r="F8" s="2">
+        <v>36327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>325</v>
+      </c>
+      <c r="D9">
+        <v>450</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>775</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>41672</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>